<commit_message>
Actualizacion de la concentracion de metricas con el proyecto viaticos_q
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/3. Medición, Monitoreo y Control/Medición/IWM_Concentración_Métricas.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/3. Medición, Monitoreo y Control/Medición/IWM_Concentración_Métricas.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Organización\Procesos\Soporte Organizacional\3. Medición, Monitoreo y Control\Medición\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="705" windowWidth="12915" windowHeight="4590" tabRatio="658" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="705" windowWidth="12915" windowHeight="4590" tabRatio="658" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Procesos" sheetId="2" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <sheet name="Esfuerzo" sheetId="6" r:id="rId5"/>
     <sheet name="Costos" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -159,10 +164,10 @@
     <t>webalgoritmia</t>
   </si>
   <si>
-    <t>&lt;Proyecto 4&gt;</t>
+    <t>Aseguramietno de la calida</t>
   </si>
   <si>
-    <t>Aseguramietno de la calida</t>
+    <t>Viaticos</t>
   </si>
 </sst>
 </file>
@@ -826,6 +831,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -833,7 +841,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -910,7 +918,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -918,6 +938,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -962,7 +987,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -984,6 +1021,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1043,7 +1085,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1051,6 +1105,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1095,7 +1154,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1117,6 +1188,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1161,7 +1237,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1183,6 +1271,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1242,7 +1335,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1250,6 +1355,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1302,12 +1412,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="131613696"/>
-        <c:axId val="50780928"/>
+        <c:axId val="129878912"/>
+        <c:axId val="129879472"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="131613696"/>
+        <c:axId val="129878912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1316,7 +1426,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50780928"/>
+        <c:crossAx val="129879472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1324,7 +1434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50780928"/>
+        <c:axId val="129879472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1335,13 +1445,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131613696"/>
+        <c:crossAx val="129878912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1359,7 +1470,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1394,17 +1505,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Productos!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
@@ -1436,7 +1536,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1444,12 +1556,12 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Productos!#REF!</c:f>
-            </c:multiLvlStrRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Productos!$O$3</c:f>
@@ -1462,21 +1574,48 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Productos!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Productos!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                  </c:multiLvlStrRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Productos!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
@@ -1508,7 +1647,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1516,6 +1667,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1529,21 +1685,33 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Productos!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Productos!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
@@ -1560,7 +1728,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1568,6 +1748,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1581,21 +1766,33 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Productos!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Productos!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
@@ -1627,7 +1824,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1635,6 +1844,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1648,21 +1862,33 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Productos!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Productos!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
@@ -1694,7 +1920,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1702,6 +1940,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1715,21 +1958,33 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Productos!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
           <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Productos!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
@@ -1746,7 +2001,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1768,6 +2035,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1781,21 +2053,33 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Productos!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
           <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Productos!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
@@ -1827,7 +2111,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1835,6 +2131,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1848,21 +2149,33 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Productos!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
           <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Productos!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
@@ -1879,7 +2192,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1901,6 +2226,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1914,6 +2244,29 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Productos!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>#REF!</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1925,12 +2278,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="133460480"/>
-        <c:axId val="52995200"/>
+        <c:axId val="129886752"/>
+        <c:axId val="131293712"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="133460480"/>
+        <c:axId val="129886752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1939,7 +2292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52995200"/>
+        <c:crossAx val="131293712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1947,7 +2300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52995200"/>
+        <c:axId val="131293712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1958,13 +2311,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133460480"/>
+        <c:crossAx val="129886752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1982,7 +2336,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2014,6 +2368,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2133,11 +2488,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="133462016"/>
-        <c:axId val="52997504"/>
+        <c:axId val="131297632"/>
+        <c:axId val="131298192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133462016"/>
+        <c:axId val="131297632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2147,7 +2502,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52997504"/>
+        <c:crossAx val="131298192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2155,7 +2510,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52997504"/>
+        <c:axId val="131298192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2167,13 +2522,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133462016"/>
+        <c:crossAx val="131297632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2191,7 +2547,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2283,7 +2639,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -2291,6 +2659,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2367,7 +2740,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -2375,6 +2760,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -2434,7 +2824,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -2442,6 +2844,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -2465,20 +2872,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="133632000"/>
-        <c:axId val="52999808"/>
+        <c:axId val="206392656"/>
+        <c:axId val="206393216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133632000"/>
+        <c:axId val="206392656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52999808"/>
+        <c:crossAx val="206393216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2486,7 +2894,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52999808"/>
+        <c:axId val="206393216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,7 +2905,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133632000"/>
+        <c:crossAx val="206392656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2706,7 +3114,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2741,7 +3149,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2953,8 +3361,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="B1:O29"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O10"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3257,8 +3665,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="B1:O41"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3800,7 +4208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -3984,8 +4392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4475,7 +4883,7 @@
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="53" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D35" s="54"/>
       <c r="E35" s="55"/>
@@ -4502,11 +4910,15 @@
       <c r="B37" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="10"/>
+      <c r="C37" s="9">
+        <v>29</v>
+      </c>
+      <c r="D37" s="10">
+        <v>27</v>
+      </c>
       <c r="E37" s="30">
         <f t="shared" ref="E37:E44" si="3">(D37-C37)</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -4516,11 +4928,15 @@
       <c r="B38" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="5"/>
+      <c r="C38" s="6">
+        <v>46</v>
+      </c>
+      <c r="D38" s="5">
+        <v>42</v>
+      </c>
       <c r="E38" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -4530,11 +4946,15 @@
       <c r="B39" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="5"/>
+      <c r="C39" s="6">
+        <v>100</v>
+      </c>
+      <c r="D39" s="5">
+        <v>20</v>
+      </c>
       <c r="E39" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -4544,11 +4964,13 @@
       <c r="B40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="6"/>
+      <c r="C40" s="6">
+        <v>8</v>
+      </c>
       <c r="D40" s="5"/>
       <c r="E40" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.3">
@@ -4558,8 +4980,12 @@
       <c r="B41" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="5"/>
+      <c r="C41" s="6">
+        <v>13</v>
+      </c>
+      <c r="D41" s="5">
+        <v>13</v>
+      </c>
       <c r="E41" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4572,9 +4998,16 @@
       <c r="B42" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="30"/>
+      <c r="C42" s="6">
+        <v>22</v>
+      </c>
+      <c r="D42" s="5">
+        <v>4</v>
+      </c>
+      <c r="E42" s="30">
+        <f t="shared" si="3"/>
+        <v>-18</v>
+      </c>
     </row>
     <row r="43" spans="1:5" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
@@ -4583,11 +5016,15 @@
       <c r="B43" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="5"/>
+      <c r="C43" s="6">
+        <v>4</v>
+      </c>
+      <c r="D43" s="5">
+        <v>1</v>
+      </c>
       <c r="E43" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="7" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -4597,11 +5034,15 @@
       <c r="B44" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="17"/>
+      <c r="C44" s="16">
+        <v>4</v>
+      </c>
+      <c r="D44" s="17">
+        <v>1</v>
+      </c>
       <c r="E44" s="31">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
   </sheetData>
@@ -4620,8 +5061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="B25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4919,7 +5360,7 @@
         <v>41206</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="42">
         <v>767.46</v>
@@ -5070,7 +5511,7 @@
         <v>18</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="5"/>
@@ -5110,7 +5551,7 @@
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="53" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D35" s="54"/>
       <c r="E35" s="55"/>
@@ -5137,11 +5578,15 @@
       <c r="B37" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="5"/>
+      <c r="C37" s="6">
+        <v>1496.9</v>
+      </c>
+      <c r="D37" s="5">
+        <v>1393.66</v>
+      </c>
       <c r="E37" s="34">
         <f t="shared" ref="E37:E44" si="3">(D37-C37)</f>
-        <v>0</v>
+        <v>-103.24000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -5151,11 +5596,15 @@
       <c r="B38" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="5"/>
+      <c r="C38" s="6">
+        <v>2745.01</v>
+      </c>
+      <c r="D38" s="5">
+        <v>2505.6</v>
+      </c>
       <c r="E38" s="34">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-239.41000000000031</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -5165,11 +5614,15 @@
       <c r="B39" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="5"/>
+      <c r="C39" s="6">
+        <v>6307.67</v>
+      </c>
+      <c r="D39" s="5">
+        <v>1261.5340000000001</v>
+      </c>
       <c r="E39" s="34">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-5046.1360000000004</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -5179,11 +5632,15 @@
       <c r="B40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="5"/>
+      <c r="C40" s="6">
+        <v>478.83</v>
+      </c>
+      <c r="D40" s="5">
+        <v>0</v>
+      </c>
       <c r="E40" s="34">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-478.83</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.3">
@@ -5193,8 +5650,12 @@
       <c r="B41" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="5"/>
+      <c r="C41" s="6">
+        <v>415.71</v>
+      </c>
+      <c r="D41" s="5">
+        <v>415.71</v>
+      </c>
       <c r="E41" s="34">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5205,13 +5666,17 @@
         <v>18</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="C42" s="6">
+        <v>703.51</v>
+      </c>
+      <c r="D42" s="5">
+        <v>127.91</v>
+      </c>
       <c r="E42" s="34">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-575.6</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -5221,11 +5686,15 @@
       <c r="B43" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="5"/>
+      <c r="C43" s="6">
+        <v>239.41</v>
+      </c>
+      <c r="D43" s="5">
+        <v>59.85</v>
+      </c>
       <c r="E43" s="34">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-179.56</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -5235,11 +5704,15 @@
       <c r="B44" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="32"/>
-      <c r="D44" s="33"/>
+      <c r="C44" s="32">
+        <v>239.41</v>
+      </c>
+      <c r="D44" s="33">
+        <v>59.85</v>
+      </c>
       <c r="E44" s="35">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-179.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion concentracion de metricas con datos de viaticos_q
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/3. Medición, Monitoreo y Control/Medición/IWM_Concentración_Métricas.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/3. Medición, Monitoreo y Control/Medición/IWM_Concentración_Métricas.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Organización\Procesos\Soporte Organizacional\3. Medición, Monitoreo y Control\Medición\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="708" windowWidth="12912" windowHeight="4596" tabRatio="658"/>
+    <workbookView xWindow="600" yWindow="705" windowWidth="12915" windowHeight="4590" tabRatio="658" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Procesos" sheetId="2" r:id="rId1"/>
@@ -14,12 +19,12 @@
     <sheet name="Esfuerzo" sheetId="6" r:id="rId5"/>
     <sheet name="Costos" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="52">
   <si>
     <t>Organizacional</t>
   </si>
@@ -136,9 +141,6 @@
   </si>
   <si>
     <t>webalgoritmia</t>
-  </si>
-  <si>
-    <t>&lt;Proyecto 4&gt;</t>
   </si>
   <si>
     <t>Aseguramietno de la calida</t>
@@ -824,6 +826,15 @@
     <xf numFmtId="14" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="5" borderId="32" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -848,6 +859,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -856,24 +876,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="5" borderId="32" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -888,6 +890,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -895,7 +900,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -972,7 +977,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -980,6 +997,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1024,7 +1046,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1046,6 +1080,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1105,7 +1144,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1113,6 +1164,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1157,7 +1213,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1179,6 +1247,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1223,7 +1296,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1245,6 +1330,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -1381,12 +1471,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="107150720"/>
-        <c:axId val="107426944"/>
+        <c:axId val="128358416"/>
+        <c:axId val="128358976"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="107150720"/>
+        <c:axId val="128358416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1395,7 +1485,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107426944"/>
+        <c:crossAx val="128358976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1403,7 +1493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107426944"/>
+        <c:axId val="128358976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1414,7 +1504,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107150720"/>
+        <c:crossAx val="128358416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1439,7 +1529,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1624,21 +1714,22 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="47302912"/>
-        <c:axId val="47312896"/>
+        <c:axId val="128361776"/>
+        <c:axId val="131060256"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="47302912"/>
+        <c:axId val="128361776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47312896"/>
+        <c:crossAx val="131060256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1646,7 +1737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47312896"/>
+        <c:axId val="131060256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1657,7 +1748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47302912"/>
+        <c:crossAx val="128361776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1682,7 +1773,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1829,11 +1920,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="107847680"/>
-        <c:axId val="107849216"/>
+        <c:axId val="131063616"/>
+        <c:axId val="131064176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107847680"/>
+        <c:axId val="131063616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1843,7 +1934,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107849216"/>
+        <c:crossAx val="131064176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1851,7 +1942,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107849216"/>
+        <c:axId val="131064176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1863,7 +1954,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107847680"/>
+        <c:crossAx val="131063616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1888,7 +1979,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1976,7 +2067,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1984,6 +2087,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2056,7 +2164,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -2064,6 +2184,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -2119,7 +2244,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -2127,6 +2264,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
@@ -2150,20 +2292,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="107947904"/>
-        <c:axId val="107949440"/>
+        <c:axId val="131068096"/>
+        <c:axId val="131068656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107947904"/>
+        <c:axId val="131068096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107949440"/>
+        <c:crossAx val="131068656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2171,7 +2314,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107949440"/>
+        <c:axId val="131068656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2182,7 +2325,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107947904"/>
+        <c:crossAx val="131068096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2391,7 +2534,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2426,7 +2569,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2638,51 +2781,51 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="B1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" customWidth="1"/>
-    <col min="3" max="3" width="56.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="12" width="16.109375" customWidth="1"/>
-    <col min="13" max="15" width="16.109375" style="6" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" customWidth="1"/>
-    <col min="17" max="17" width="16.6640625" style="6" customWidth="1"/>
-    <col min="18" max="18" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="56.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="15" width="16.140625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" style="6" customWidth="1"/>
+    <col min="18" max="18" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="44" t="s">
+    <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="44" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47" t="s">
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="51"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="48"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="55"/>
+      <c r="N1" s="56"/>
       <c r="O1" s="57"/>
-      <c r="P1" s="50" t="s">
+      <c r="P1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="51"/>
-    </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="Q1" s="54"/>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="35">
@@ -2729,7 +2872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="11">
         <v>1</v>
       </c>
@@ -2758,12 +2901,12 @@
       <c r="O3" s="36"/>
       <c r="P3" s="36"/>
       <c r="Q3" s="36"/>
-      <c r="R3" s="59">
+      <c r="R3" s="45">
         <f>AVERAGE(D3:O3)</f>
         <v>0.83340833333333342</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -2796,12 +2939,12 @@
       <c r="O4" s="36"/>
       <c r="P4" s="36"/>
       <c r="Q4" s="36"/>
-      <c r="R4" s="59">
+      <c r="R4" s="45">
         <f>AVERAGE(D4:O4)</f>
         <v>0.75097045454545452</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="11">
         <v>3</v>
       </c>
@@ -2828,12 +2971,12 @@
       <c r="O5" s="36"/>
       <c r="P5" s="36"/>
       <c r="Q5" s="36"/>
-      <c r="R5" s="59" t="e">
-        <f t="shared" ref="R5:R9" si="0">AVERAGE(D5:O5)</f>
+      <c r="R5" s="45" t="e">
+        <f t="shared" ref="R5:R7" si="0">AVERAGE(D5:O5)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -2860,12 +3003,12 @@
       <c r="O6" s="36"/>
       <c r="P6" s="36"/>
       <c r="Q6" s="36"/>
-      <c r="R6" s="59" t="e">
+      <c r="R6" s="45" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
         <v>5</v>
       </c>
@@ -2886,12 +3029,12 @@
       <c r="O7" s="36"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="36"/>
-      <c r="R7" s="59" t="e">
+      <c r="R7" s="45" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -2914,12 +3057,12 @@
       <c r="O8" s="36"/>
       <c r="P8" s="36"/>
       <c r="Q8" s="36"/>
-      <c r="R8" s="59">
+      <c r="R8" s="45">
         <f>AVERAGE(D8:O8)</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <v>7</v>
       </c>
@@ -2942,17 +3085,17 @@
         <v>0.46153846153846156</v>
       </c>
       <c r="Q9" s="36"/>
-      <c r="R9" s="59">
+      <c r="R9" s="45">
         <f>AVERAGE(P9:Q9)</f>
         <v>0.46153846153846156</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="11">
         <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="36"/>
       <c r="E10" s="36"/>
@@ -2970,17 +3113,17 @@
         <v>0.5</v>
       </c>
       <c r="Q10" s="36"/>
-      <c r="R10" s="59">
+      <c r="R10" s="45">
         <f t="shared" ref="R10:R11" si="1">AVERAGE(P10:Q10)</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
         <v>9</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="36"/>
@@ -2998,12 +3141,12 @@
         <v>0.7</v>
       </c>
       <c r="Q11" s="36"/>
-      <c r="R11" s="59">
+      <c r="R11" s="45">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
     </row>
-    <row r="28" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="D1:F1"/>
@@ -3023,51 +3166,51 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="B1:R41"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" customWidth="1"/>
-    <col min="3" max="3" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
-    <col min="13" max="15" width="11.5546875" style="6"/>
-    <col min="18" max="18" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="13" max="15" width="11.5703125" style="6"/>
+    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="44" t="str">
+    <row r="1" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="47" t="str">
         <f>Procesos!D1</f>
         <v>Web IWM</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="44" t="str">
+      <c r="E1" s="48"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="47" t="str">
         <f>Procesos!G1</f>
         <v>Web Anwar</v>
       </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="44" t="str">
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="47" t="str">
         <f>Procesos!J1</f>
         <v>Inter_cabina</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="45" t="s">
+      <c r="K1" s="48"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="48"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="46"/>
-    </row>
-    <row r="2" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q1" s="49"/>
+    </row>
+    <row r="2" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="25">
@@ -3126,12 +3269,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="11">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="36">
         <v>1</v>
@@ -3155,17 +3298,17 @@
       <c r="O3" s="36"/>
       <c r="P3" s="36"/>
       <c r="Q3" s="36"/>
-      <c r="R3" s="59">
+      <c r="R3" s="45">
         <f>AVERAGE(D3:Q3)</f>
         <v>0.80909999999999993</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="11">
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="36" t="s">
         <v>23</v>
@@ -3191,12 +3334,12 @@
       <c r="O4" s="36"/>
       <c r="P4" s="36"/>
       <c r="Q4" s="36"/>
-      <c r="R4" s="59">
-        <f t="shared" ref="R4:R10" si="0">AVERAGE(D4:Q4)</f>
+      <c r="R4" s="45">
+        <f t="shared" ref="R4:R8" si="0">AVERAGE(D4:Q4)</f>
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="11">
         <v>3</v>
       </c>
@@ -3227,12 +3370,12 @@
       <c r="O5" s="36"/>
       <c r="P5" s="36"/>
       <c r="Q5" s="36"/>
-      <c r="R5" s="59">
+      <c r="R5" s="45">
         <f t="shared" si="0"/>
         <v>0.78175714285714282</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -3263,17 +3406,17 @@
       <c r="O6" s="36"/>
       <c r="P6" s="36"/>
       <c r="Q6" s="36"/>
-      <c r="R6" s="59">
+      <c r="R6" s="45">
         <f t="shared" si="0"/>
         <v>0.58695652173913049</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="36"/>
@@ -3291,17 +3434,17 @@
       <c r="O7" s="36"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="36"/>
-      <c r="R7" s="59">
+      <c r="R7" s="45">
         <f t="shared" si="0"/>
         <v>0.66669999999999996</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <v>6</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="36"/>
       <c r="E8" s="36"/>
@@ -3317,17 +3460,17 @@
       <c r="O8" s="36"/>
       <c r="P8" s="36"/>
       <c r="Q8" s="36"/>
-      <c r="R8" s="59" t="e">
+      <c r="R8" s="45" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="36"/>
       <c r="E9" s="36"/>
@@ -3343,12 +3486,12 @@
       <c r="O9" s="36"/>
       <c r="P9" s="36"/>
       <c r="Q9" s="36"/>
-      <c r="R9" s="59" t="e">
+      <c r="R9" s="45" t="e">
         <f>AVERAGE(P9:Q9)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -3371,17 +3514,17 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="Q10" s="36"/>
-      <c r="R10" s="59">
+      <c r="R10" s="45">
         <f>AVERAGE(P10:Q10)</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
         <v>9</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="36"/>
@@ -3399,17 +3542,17 @@
         <v>0.9</v>
       </c>
       <c r="Q11" s="36"/>
-      <c r="R11" s="59">
+      <c r="R11" s="45">
         <f t="shared" ref="R11:R13" si="1">AVERAGE(P11:Q11)</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
         <v>10</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="36"/>
@@ -3427,17 +3570,17 @@
         <v>0.94117647058823528</v>
       </c>
       <c r="Q12" s="36"/>
-      <c r="R12" s="59">
+      <c r="R12" s="45">
         <f t="shared" si="1"/>
         <v>0.94117647058823528</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="36"/>
       <c r="E13" s="36"/>
@@ -3455,57 +3598,57 @@
         <v>1</v>
       </c>
       <c r="Q13" s="36"/>
-      <c r="R13" s="59">
+      <c r="R13" s="45">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C16" s="6"/>
     </row>
-    <row r="33" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="6" t="s">
         <v>29</v>
       </c>
@@ -3531,47 +3674,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P28"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="N3" sqref="N3:N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="11.5546875" style="6"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="11.5703125" style="6"/>
     <col min="16" max="16" width="21" customWidth="1"/>
-    <col min="18" max="18" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="D1" s="44" t="str">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D1" s="47" t="str">
         <f>Procesos!D1</f>
         <v>Web IWM</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="44" t="str">
+      <c r="E1" s="48"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="47" t="str">
         <f>Procesos!G1</f>
         <v>Web Anwar</v>
       </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="44" t="str">
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="47" t="str">
         <f>Procesos!J1</f>
         <v>Inter_cabina</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46"/>
-    </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="K1" s="48"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="48"/>
+      <c r="O1" s="49"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="25">
@@ -3623,7 +3766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11">
         <v>1</v>
       </c>
@@ -3647,19 +3790,19 @@
         <v>1</v>
       </c>
       <c r="L3" s="39"/>
-      <c r="M3" s="58">
+      <c r="M3" s="44">
         <v>0.5</v>
       </c>
-      <c r="N3" s="58">
+      <c r="N3" s="44">
         <v>0</v>
       </c>
-      <c r="O3" s="58"/>
-      <c r="P3" s="59">
+      <c r="O3" s="44"/>
+      <c r="P3" s="45">
         <f>AVERAGE(D3:O3)</f>
         <v>0.3611166666666667</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -3685,19 +3828,19 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="L4" s="39"/>
-      <c r="M4" s="58">
+      <c r="M4" s="44">
         <v>0.33333333333333331</v>
       </c>
-      <c r="N4" s="58">
+      <c r="N4" s="44">
         <v>0.66666666666666663</v>
       </c>
-      <c r="O4" s="58"/>
-      <c r="P4" s="59">
+      <c r="O4" s="44"/>
+      <c r="P4" s="45">
         <f>AVERAGE(D4:O4)</f>
         <v>0.66666190476190479</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="11">
         <v>3</v>
       </c>
@@ -3721,22 +3864,22 @@
       </c>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="59" t="e">
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="45" t="e">
         <f>AVERAGE(D5:O5)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="D6" s="37"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
     </row>
-    <row r="28" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D1:F1"/>
@@ -3754,49 +3897,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P28"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="4" max="4" width="10" style="38" customWidth="1"/>
     <col min="5" max="12" width="10" customWidth="1"/>
     <col min="13" max="15" width="10" style="6" customWidth="1"/>
     <col min="16" max="16" width="19" customWidth="1"/>
     <col min="17" max="17" width="10" customWidth="1"/>
-    <col min="18" max="18" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="D1" s="44" t="str">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D1" s="47" t="str">
         <f>Procesos!D1</f>
         <v>Web IWM</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="44" t="str">
+      <c r="E1" s="48"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="47" t="str">
         <f>Procesos!G1</f>
         <v>Web Anwar</v>
       </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="44" t="str">
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="47" t="str">
         <f>Procesos!J1</f>
         <v>Inter_cabina</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46"/>
-    </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="K1" s="48"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="48"/>
+      <c r="O1" s="49"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="25">
@@ -3848,7 +3991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="11">
         <v>1</v>
       </c>
@@ -3874,19 +4017,19 @@
         <v>0</v>
       </c>
       <c r="L3" s="39"/>
-      <c r="M3" s="60">
+      <c r="M3" s="46">
         <v>0</v>
       </c>
-      <c r="N3" s="58">
+      <c r="N3" s="44">
         <v>0.25</v>
       </c>
-      <c r="O3" s="58"/>
-      <c r="P3" s="59">
+      <c r="O3" s="44"/>
+      <c r="P3" s="45">
         <f>AVERAGE(D3:L3)</f>
         <v>0.35</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -3912,19 +4055,19 @@
         <v>0.2</v>
       </c>
       <c r="L4" s="39"/>
-      <c r="M4" s="60">
+      <c r="M4" s="46">
         <v>0.5</v>
       </c>
-      <c r="N4" s="58">
+      <c r="N4" s="44">
         <v>0.5</v>
       </c>
-      <c r="O4" s="58"/>
-      <c r="P4" s="59">
+      <c r="O4" s="44"/>
+      <c r="P4" s="45">
         <f t="shared" ref="P4:P5" si="0">AVERAGE(D4:L4)</f>
         <v>0.35833333333333334</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="11">
         <v>3</v>
       </c>
@@ -3946,22 +4089,22 @@
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="59" t="e">
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="45" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="D6" s="37"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
     </row>
-    <row r="28" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D1:F1"/>
@@ -3979,28 +4122,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.44140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="6"/>
+    <col min="1" max="1" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="6"/>
     <col min="5" max="5" width="11" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
-    </row>
-    <row r="3" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
+    </row>
+    <row r="3" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="21" t="s">
         <v>34</v>
@@ -4163,13 +4306,13 @@
       <c r="B12" s="28"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="54"/>
-    </row>
-    <row r="14" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="59"/>
+      <c r="E13" s="60"/>
+    </row>
+    <row r="14" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="21" t="s">
         <v>34</v>
@@ -4328,15 +4471,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="52" t="s">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="53"/>
-      <c r="E24" s="54"/>
-    </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="59"/>
+      <c r="E24" s="60"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="21" t="s">
         <v>34</v>
@@ -4351,7 +4494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="40">
         <v>41193</v>
       </c>
@@ -4369,7 +4512,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>
@@ -4383,7 +4526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>16</v>
       </c>
@@ -4397,7 +4540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>16</v>
       </c>
@@ -4411,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>16</v>
       </c>
@@ -4439,7 +4582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>16</v>
       </c>
@@ -4453,7 +4596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>16</v>
       </c>
@@ -4467,15 +4610,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="53"/>
-      <c r="E35" s="54"/>
-    </row>
-    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="59"/>
+      <c r="E35" s="60"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="21" t="s">
         <v>34</v>
@@ -4490,71 +4633,89 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
+      <c r="C37" s="8">
+        <v>29</v>
+      </c>
+      <c r="D37" s="9">
+        <v>27</v>
+      </c>
       <c r="E37" s="29">
         <f t="shared" ref="E37:E44" si="3">(D37-C37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="4"/>
+      <c r="C38" s="5">
+        <v>46</v>
+      </c>
+      <c r="D38" s="4">
+        <v>42</v>
+      </c>
       <c r="E38" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="4"/>
+      <c r="C39" s="5">
+        <v>100</v>
+      </c>
+      <c r="D39" s="4">
+        <v>20</v>
+      </c>
       <c r="E39" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="5"/>
+      <c r="C40" s="5">
+        <v>8</v>
+      </c>
       <c r="D40" s="4"/>
       <c r="E40" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="4"/>
+      <c r="C41" s="5">
+        <v>13</v>
+      </c>
+      <c r="D41" s="4">
+        <v>13</v>
+      </c>
       <c r="E41" s="29">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4567,36 +4728,51 @@
       <c r="B42" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="29"/>
-    </row>
-    <row r="43" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="5">
+        <v>22</v>
+      </c>
+      <c r="D42" s="4">
+        <v>4</v>
+      </c>
+      <c r="E42" s="29">
+        <f t="shared" si="3"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="4"/>
+      <c r="C43" s="5">
+        <v>4</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1</v>
+      </c>
       <c r="E43" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="16"/>
+      <c r="C44" s="5">
+        <v>4</v>
+      </c>
+      <c r="D44" s="16">
+        <v>1</v>
+      </c>
       <c r="E44" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
   </sheetData>
@@ -4615,29 +4791,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="6"/>
-    <col min="2" max="2" width="34.44140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="6"/>
-    <col min="5" max="5" width="14.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.44140625" style="6"/>
+    <col min="1" max="1" width="11.42578125" style="6"/>
+    <col min="2" max="2" width="34.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="6"/>
+    <col min="5" max="5" width="14.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
-    </row>
-    <row r="3" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
+    </row>
+    <row r="3" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="11" t="s">
         <v>34</v>
@@ -4798,13 +4974,13 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="54"/>
-    </row>
-    <row r="14" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="59"/>
+      <c r="E13" s="60"/>
+    </row>
+    <row r="14" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="11" t="s">
         <v>34</v>
@@ -4914,7 +5090,7 @@
         <v>41206</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="41">
         <v>767.46</v>
@@ -4963,15 +5139,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="52" t="s">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="53"/>
-      <c r="E24" s="54"/>
-    </row>
-    <row r="25" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="59"/>
+      <c r="E24" s="60"/>
+    </row>
+    <row r="25" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="11" t="s">
         <v>34</v>
@@ -4986,7 +5162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="43">
         <v>41194</v>
       </c>
@@ -5004,7 +5180,7 @@
         <v>-206.48000000000013</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>
@@ -5018,7 +5194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>16</v>
       </c>
@@ -5032,7 +5208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>16</v>
       </c>
@@ -5046,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>16</v>
       </c>
@@ -5065,7 +5241,7 @@
         <v>16</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="4"/>
@@ -5074,7 +5250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>16</v>
       </c>
@@ -5088,7 +5264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>16</v>
       </c>
@@ -5102,15 +5278,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="53"/>
-      <c r="E35" s="54"/>
-    </row>
-    <row r="36" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="59"/>
+      <c r="E35" s="60"/>
+    </row>
+    <row r="36" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="11" t="s">
         <v>34</v>
@@ -5125,71 +5301,91 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="4"/>
+      <c r="C37" s="5">
+        <v>1496.9</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1393.66</v>
+      </c>
       <c r="E37" s="33">
         <f t="shared" ref="E37:E44" si="3">(D37-C37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-103.24000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="4"/>
+      <c r="C38" s="5">
+        <v>2745.01</v>
+      </c>
+      <c r="D38" s="4">
+        <v>2505.6</v>
+      </c>
       <c r="E38" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-239.41000000000031</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="4"/>
+      <c r="C39" s="5">
+        <v>6307.67</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1261.5340000000001</v>
+      </c>
       <c r="E39" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-5046.1360000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="4"/>
+      <c r="C40" s="5">
+        <v>478.83</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0</v>
+      </c>
       <c r="E40" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-478.83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="4"/>
+      <c r="C41" s="5">
+        <v>415.71</v>
+      </c>
+      <c r="D41" s="4">
+        <v>415.71</v>
+      </c>
       <c r="E41" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5200,41 +5396,53 @@
         <v>16</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="C42" s="5">
+        <v>703.51</v>
+      </c>
+      <c r="D42" s="4">
+        <v>127.91</v>
+      </c>
       <c r="E42" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-575.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="4"/>
+      <c r="C43" s="5">
+        <v>239.41</v>
+      </c>
+      <c r="D43" s="4">
+        <v>59.85</v>
+      </c>
       <c r="E43" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>-179.56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="31"/>
-      <c r="D44" s="32"/>
+      <c r="C44" s="5">
+        <v>239.41</v>
+      </c>
+      <c r="D44" s="4">
+        <v>59.85</v>
+      </c>
       <c r="E44" s="34">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-179.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Anexo comentario a error
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/3. Medición, Monitoreo y Control/Medición/IWM_Concentración_Métricas.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/3. Medición, Monitoreo y Control/Medición/IWM_Concentración_Métricas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="705" windowWidth="12915" windowHeight="4590" tabRatio="658" activeTab="5"/>
+    <workbookView xWindow="600" yWindow="705" windowWidth="12915" windowHeight="4590" tabRatio="658" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Procesos" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="52">
   <si>
     <t>Organizacional</t>
   </si>
@@ -978,9 +978,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1047,9 +1045,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1145,9 +1141,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1214,9 +1208,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1297,9 +1289,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1471,12 +1461,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="128358416"/>
-        <c:axId val="128358976"/>
+        <c:axId val="103431424"/>
+        <c:axId val="103431984"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="128358416"/>
+        <c:axId val="103431424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,7 +1475,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128358976"/>
+        <c:crossAx val="103431984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1493,7 +1483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128358976"/>
+        <c:axId val="103431984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1504,14 +1494,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128358416"/>
+        <c:crossAx val="103431424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1714,12 +1703,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="128361776"/>
-        <c:axId val="131060256"/>
+        <c:axId val="119250752"/>
+        <c:axId val="119251312"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="128361776"/>
+        <c:axId val="119250752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1729,7 +1718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131060256"/>
+        <c:crossAx val="119251312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1737,7 +1726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131060256"/>
+        <c:axId val="119251312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1748,14 +1737,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128361776"/>
+        <c:crossAx val="119250752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1800,7 +1788,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1920,11 +1907,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="131063616"/>
-        <c:axId val="131064176"/>
+        <c:axId val="119254672"/>
+        <c:axId val="119255232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="131063616"/>
+        <c:axId val="119254672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1934,7 +1921,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131064176"/>
+        <c:crossAx val="119255232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1942,7 +1929,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131064176"/>
+        <c:axId val="119255232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1954,14 +1941,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131063616"/>
+        <c:crossAx val="119254672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2006,7 +1992,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2068,9 +2053,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2165,9 +2148,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2245,9 +2226,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2292,11 +2271,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="131068096"/>
-        <c:axId val="131068656"/>
+        <c:axId val="119777312"/>
+        <c:axId val="119777872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="131068096"/>
+        <c:axId val="119777312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2306,7 +2285,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131068656"/>
+        <c:crossAx val="119777872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2314,7 +2293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131068656"/>
+        <c:axId val="119777872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2325,14 +2304,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131068096"/>
+        <c:crossAx val="119777312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4123,7 +4101,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4634,8 +4612,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="11" t="s">
-        <v>16</v>
+      <c r="A37" s="43">
+        <v>42194</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>1</v>
@@ -4652,8 +4630,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
-        <v>16</v>
+      <c r="A38" s="43">
+        <v>42201</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>20</v>
@@ -4680,11 +4658,11 @@
         <v>100</v>
       </c>
       <c r="D39" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E39" s="29">
         <f t="shared" si="3"/>
-        <v>-80</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -4697,15 +4675,17 @@
       <c r="C40" s="5">
         <v>8</v>
       </c>
-      <c r="D40" s="4"/>
+      <c r="D40" s="4">
+        <v>0</v>
+      </c>
       <c r="E40" s="29">
         <f t="shared" si="3"/>
         <v>-8</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.3">
-      <c r="A41" s="11" t="s">
-        <v>16</v>
+      <c r="A41" s="43">
+        <v>42202</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>21</v>
@@ -4714,16 +4694,16 @@
         <v>13</v>
       </c>
       <c r="D41" s="4">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E41" s="29">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
-        <v>16</v>
+      <c r="A42" s="43">
+        <v>42202</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>37</v>
@@ -4732,16 +4712,16 @@
         <v>22</v>
       </c>
       <c r="D42" s="4">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E42" s="29">
         <f t="shared" si="3"/>
-        <v>-18</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="11" t="s">
-        <v>16</v>
+      <c r="A43" s="43">
+        <v>42202</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>14</v>
@@ -4750,16 +4730,16 @@
         <v>4</v>
       </c>
       <c r="D43" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E43" s="29">
         <f t="shared" si="3"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="11" t="s">
-        <v>16</v>
+      <c r="A44" s="43">
+        <v>42202</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>15</v>
@@ -4768,11 +4748,11 @@
         <v>4</v>
       </c>
       <c r="D44" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" s="30">
         <f t="shared" si="3"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
   </sheetData>
@@ -4791,13 +4771,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="6"/>
+    <col min="1" max="1" width="14.5703125" style="6" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="6"/>
@@ -5302,8 +5282,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="11" t="s">
-        <v>16</v>
+      <c r="A37" s="43">
+        <v>42194</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>1</v>
@@ -5320,8 +5300,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
-        <v>16</v>
+      <c r="A38" s="43">
+        <v>42201</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>20</v>
@@ -5348,11 +5328,11 @@
         <v>6307.67</v>
       </c>
       <c r="D39" s="4">
-        <v>1261.5340000000001</v>
+        <v>0</v>
       </c>
       <c r="E39" s="33">
         <f t="shared" si="3"/>
-        <v>-5046.1360000000004</v>
+        <v>-6307.67</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -5374,8 +5354,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.3">
-      <c r="A41" s="11" t="s">
-        <v>16</v>
+      <c r="A41" s="43">
+        <v>42202</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>21</v>
@@ -5384,16 +5364,16 @@
         <v>415.71</v>
       </c>
       <c r="D41" s="4">
-        <v>415.71</v>
+        <v>207.85</v>
       </c>
       <c r="E41" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-207.85999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
-        <v>16</v>
+      <c r="A42" s="43">
+        <v>42202</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>39</v>
@@ -5402,16 +5382,16 @@
         <v>703.51</v>
       </c>
       <c r="D42" s="4">
-        <v>127.91</v>
+        <v>351.75</v>
       </c>
       <c r="E42" s="33">
         <f t="shared" si="3"/>
-        <v>-575.6</v>
+        <v>-351.76</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="11" t="s">
-        <v>16</v>
+      <c r="A43" s="43">
+        <v>42202</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>14</v>
@@ -5419,17 +5399,17 @@
       <c r="C43" s="5">
         <v>239.41</v>
       </c>
-      <c r="D43" s="4">
-        <v>59.85</v>
+      <c r="D43" s="6">
+        <v>119.7</v>
       </c>
       <c r="E43" s="33">
         <f t="shared" si="3"/>
-        <v>-179.56</v>
+        <v>-119.71</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="11" t="s">
-        <v>16</v>
+      <c r="A44" s="43">
+        <v>42202</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>15</v>
@@ -5437,12 +5417,12 @@
       <c r="C44" s="5">
         <v>239.41</v>
       </c>
-      <c r="D44" s="4">
-        <v>59.85</v>
+      <c r="D44" s="6">
+        <v>119.7</v>
       </c>
       <c r="E44" s="34">
         <f t="shared" si="3"/>
-        <v>-179.56</v>
+        <v>-119.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>